<commit_message>
Creacion de archivos csv
</commit_message>
<xml_diff>
--- a/Datos/quincena.xlsx
+++ b/Datos/quincena.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeadHunters\Desktop\Documents\GitHub\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4CDF2ED-2B2B-4D20-A288-905069289C1E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0DAD5ACF-287E-4376-A5B8-3DE7DE8653BF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{5C687F13-986D-4358-82FD-E2A7EB9C45C1}"/>
   </bookViews>
@@ -25,12 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>2018-04-22</t>
   </si>
   <si>
     <t>2018-05-07</t>
+  </si>
+  <si>
+    <t>idquincena</t>
+  </si>
+  <si>
+    <t>inicio</t>
+  </si>
+  <si>
+    <t>fin</t>
   </si>
 </sst>
 </file>
@@ -66,10 +75,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -386,29 +398,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C870CA-9F9B-4CC1-8EE1-43F53925E74F}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -490,6 +508,11 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se agregan atributos a Quincena, y sus registros respectivos
</commit_message>
<xml_diff>
--- a/Datos/quincena.xlsx
+++ b/Datos/quincena.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeadHunters\Desktop\Documents\GitHub\proyecto\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\iso\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0DAD5ACF-287E-4376-A5B8-3DE7DE8653BF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046FB6A6-39AA-47E3-BC95-D9BCFEA05E22}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{5C687F13-986D-4358-82FD-E2A7EB9C45C1}"/>
   </bookViews>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>2018-04-22</t>
-  </si>
-  <si>
-    <t>2018-05-07</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
   <si>
     <t>idquincena</t>
   </si>
@@ -40,6 +34,108 @@
   </si>
   <si>
     <t>fin</t>
+  </si>
+  <si>
+    <t>31/04/2018</t>
+  </si>
+  <si>
+    <t>31/06/2018</t>
+  </si>
+  <si>
+    <t>31/09/2018</t>
+  </si>
+  <si>
+    <t>31/11/2018</t>
+  </si>
+  <si>
+    <t>quincenareportada</t>
+  </si>
+  <si>
+    <t>2018-1</t>
+  </si>
+  <si>
+    <t>2018-2</t>
+  </si>
+  <si>
+    <t>2018-3</t>
+  </si>
+  <si>
+    <t>2018-4</t>
+  </si>
+  <si>
+    <t>2018-5</t>
+  </si>
+  <si>
+    <t>2018-6</t>
+  </si>
+  <si>
+    <t>2018-7</t>
+  </si>
+  <si>
+    <t>2018-8</t>
+  </si>
+  <si>
+    <t>2018-9</t>
+  </si>
+  <si>
+    <t>2018-10</t>
+  </si>
+  <si>
+    <t>2018-11</t>
+  </si>
+  <si>
+    <t>2018-12</t>
+  </si>
+  <si>
+    <t>2018-13</t>
+  </si>
+  <si>
+    <t>2018-14</t>
+  </si>
+  <si>
+    <t>2018-15</t>
+  </si>
+  <si>
+    <t>2018-16</t>
+  </si>
+  <si>
+    <t>2018-17</t>
+  </si>
+  <si>
+    <t>2018-18</t>
+  </si>
+  <si>
+    <t>2018-19</t>
+  </si>
+  <si>
+    <t>2018-20</t>
+  </si>
+  <si>
+    <t>2018-21</t>
+  </si>
+  <si>
+    <t>2018-22</t>
+  </si>
+  <si>
+    <t>2018-23</t>
+  </si>
+  <si>
+    <t>2018-24</t>
+  </si>
+  <si>
+    <t>quincenaenqueseraprocesada</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>habil</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>TRUE</t>
   </si>
 </sst>
 </file>
@@ -75,13 +171,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -398,120 +499,519 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C870CA-9F9B-4CC1-8EE1-43F53925E74F}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>43101</v>
+      </c>
+      <c r="C2" s="3">
+        <v>43115</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>43116</v>
+      </c>
+      <c r="C3" s="3">
+        <v>43131</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B4" s="3">
+        <v>43132</v>
+      </c>
+      <c r="C4" s="3">
+        <v>43146</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="B5" s="3">
+        <v>43147</v>
+      </c>
+      <c r="C5" s="3">
+        <v>43159</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>43160</v>
+      </c>
+      <c r="C6" s="3">
+        <v>43174</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>43175</v>
+      </c>
+      <c r="C7" s="3">
+        <v>43190</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>43191</v>
+      </c>
+      <c r="C8" s="3">
+        <v>43205</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>43206</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>43221</v>
+      </c>
+      <c r="C10" s="3">
+        <v>43235</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C11" s="3">
+        <v>43251</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>43252</v>
+      </c>
+      <c r="C12" s="3">
+        <v>43266</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>43267</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>43282</v>
+      </c>
+      <c r="C14" s="3">
+        <v>43296</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>43297</v>
+      </c>
+      <c r="C15" s="3">
+        <v>43312</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>43313</v>
+      </c>
+      <c r="C16" s="3">
+        <v>43327</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>43328</v>
+      </c>
+      <c r="C17" s="3">
+        <v>43343</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>43344</v>
+      </c>
+      <c r="C18" s="3">
+        <v>43358</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3">
+        <v>43359</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3">
+        <v>43374</v>
+      </c>
+      <c r="C20" s="3">
+        <v>43388</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3">
+        <v>43389</v>
+      </c>
+      <c r="C21" s="3">
+        <v>43404</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3">
+        <v>43405</v>
+      </c>
+      <c r="C22" s="3">
+        <v>43419</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3">
+        <v>43420</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3">
+        <v>43435</v>
+      </c>
+      <c r="C24" s="3">
+        <v>43449</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3">
+        <v>43450</v>
+      </c>
+      <c r="C25" s="3">
+        <v>43465</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>